<commit_message>
annotated training schedule draft
</commit_message>
<xml_diff>
--- a/resources/acronyms.xlsx
+++ b/resources/acronyms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Dropbox\g2sq\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B69B981-B781-4AC0-A8F2-FE2F32B52FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93185AD-5275-4BB7-8254-4E64B099B2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5F610E7D-516F-4D0E-9C99-25E102E12365}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>acronym</t>
   </si>
@@ -104,6 +104,18 @@
   </si>
   <si>
     <t>Quality Asssurance</t>
+  </si>
+  <si>
+    <t>ToC</t>
+  </si>
+  <si>
+    <t>Table of Content</t>
+  </si>
+  <si>
+    <t>HIES</t>
+  </si>
+  <si>
+    <t>Household Income and Expenditure Survey</t>
   </si>
 </sst>
 </file>
@@ -455,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCDB658-A979-4647-B5F9-26FDB723BC77}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,6 +574,22 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new call out boxes
</commit_message>
<xml_diff>
--- a/resources/acronyms.xlsx
+++ b/resources/acronyms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Dropbox\g2sq\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93185AD-5275-4BB7-8254-4E64B099B2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72151FC-7B43-4F36-996A-CE4145106DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5F610E7D-516F-4D0E-9C99-25E102E12365}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>acronym</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>Household Income and Expenditure Survey</t>
+  </si>
+  <si>
+    <t>CAWI</t>
+  </si>
+  <si>
+    <t>Computer Assissted Web Interviewing</t>
   </si>
 </sst>
 </file>
@@ -467,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCDB658-A979-4647-B5F9-26FDB723BC77}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -590,6 +596,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>